<commit_message>
data file and pom.xml changes
</commit_message>
<xml_diff>
--- a/data/ExcelUtil.xlsx
+++ b/data/ExcelUtil.xlsx
@@ -63,10 +63,10 @@
     <t>abhijeet</t>
   </si>
   <si>
-    <t>abhijit291@gmail.com</t>
-  </si>
-  <si>
     <t>abhijit204@gmail.com</t>
+  </si>
+  <si>
+    <t>abhiit291@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -506,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -520,7 +520,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>